<commit_message>
Changes done for Kaman new UI - header & footer
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\Kaman_ECTEST_Sanity\Input_files\Actual_testcases\Kaman\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9809810E-BD82-4A1E-9513-CF29B4807361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E13B91-C165-43A2-AFFB-20968BB8202E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>TestCase</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>CSS</t>
+  </si>
+  <si>
+    <t>EleType1</t>
+  </si>
+  <si>
+    <t>EleType2</t>
+  </si>
+  <si>
+    <t>JSElement</t>
   </si>
 </sst>
 </file>
@@ -487,14 +496,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+      <selection activeCell="A3" sqref="A3:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
   </cols>
@@ -583,10 +592,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -615,7 +624,7 @@
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="b">
+      <c r="B3" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -623,7 +632,7 @@
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="b">
+      <c r="B4" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -631,8 +640,24 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="b">
+      <c r="B5" s="3" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -653,12 +678,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -855,6 +874,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
@@ -864,15 +889,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -889,4 +905,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TC01 Dom changes ECTEST
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E13B91-C165-43A2-AFFB-20968BB8202E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B189EFA4-3292-4FDA-BF60-BB6C4AABE06C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_Verify_HomePage" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>KamanLogo</t>
   </si>
   <si>
-    <t>HomeCarousel</t>
-  </si>
-  <si>
     <t>SearchBoxHomePage</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>JSElement</t>
+  </si>
+  <si>
+    <t>HeroBanner</t>
   </si>
 </sst>
 </file>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -541,13 +541,13 @@
     <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>10</v>
@@ -556,31 +556,31 @@
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -617,7 +617,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -630,7 +630,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>1</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -646,18 +646,18 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -669,15 +669,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -874,6 +865,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -881,14 +881,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -907,6 +899,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
ECTEST Sanity Testcases Update
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B189EFA4-3292-4FDA-BF60-BB6C4AABE06C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_Verify_HomePage" sheetId="1" r:id="rId1"/>
@@ -77,13 +71,13 @@
     <t>JSElement</t>
   </si>
   <si>
-    <t>HeroBanner</t>
+    <t>Herobanner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -492,11 +486,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -591,11 +585,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -662,13 +656,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://192.168.15.18/storeus" xr:uid="{C28EA635-1DD4-4B93-B594-513E4D966091}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://192.168.15.18/storeus"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -865,7 +865,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -874,13 +874,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -899,19 +902,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test for git integration
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC01_Verify_HomePage.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kaman_Multisite\Automation\KAMAN_ECTEST_IE_SANITY-master\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_Verify_HomePage" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>TestCase</t>
   </si>
@@ -72,6 +77,9 @@
   </si>
   <si>
     <t>Herobanner</t>
+  </si>
+  <si>
+    <t>WAIT</t>
   </si>
 </sst>
 </file>
@@ -487,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -535,17 +543,11 @@
     <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
@@ -553,13 +555,13 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -568,12 +570,27 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -669,6 +686,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -865,15 +891,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
@@ -884,6 +901,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -900,12 +925,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>